<commit_message>
Code BT13, BT14, BT15, BT16 BT13: TẠO TESTLISTENER CHO PROJECT BT14: SỬ DỤNG LOG4J ĐỂ GHI LOG VÀO FILE BT15. TẠO EXTENT REPORT Bt16. TẠO ALLURE REPORT
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataCRM.xlsx
+++ b/src/test/resources/testdata/DataCRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\AUTOTEST\BAITAP\BT_SeleniumMavenTestNGParallel122025\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0859EB9-B7C0-42C3-BFF4-EFCE93612ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697C6873-2CB2-4AFE-B260-053AEE7F4FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>EMAIL</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Hstest</t>
+  </si>
+  <si>
+    <t>Yến Nhi 2</t>
   </si>
 </sst>
 </file>
@@ -729,10 +732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -874,6 +877,71 @@
         <v>48</v>
       </c>
     </row>
+    <row r="3" spans="1:21" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="4">
+        <v>982198605</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="6">
+        <v>45971</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -885,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFD65A5-8281-4929-9BFC-350F5C985989}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>